<commit_message>
made some examples how it would work
</commit_message>
<xml_diff>
--- a/src/main/resources/data/data.xlsx
+++ b/src/main/resources/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ДИПЛОМ\SpringDiploma\ustu\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DC7160-4679-416F-9DD8-72350D2E3526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8DFA3D-5A8B-4694-8A64-14A3012B766D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="1572" windowWidth="17280" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,41 +25,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>middlename</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>telephone</t>
-  </si>
-  <si>
     <t>6 card id</t>
   </si>
   <si>
     <t>8 card id</t>
   </si>
   <si>
-    <t>post</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>ru passport</t>
-  </si>
-  <si>
     <t>Антон</t>
   </si>
   <si>
@@ -141,9 +117,6 @@
     <t>ул. Дзержинсокго</t>
   </si>
   <si>
-    <t>street</t>
-  </si>
-  <si>
     <t>пр. Ленина</t>
   </si>
   <si>
@@ -172,6 +145,63 @@
   </si>
   <si>
     <t>женщина</t>
+  </si>
+  <si>
+    <t>Стажёр</t>
+  </si>
+  <si>
+    <t>Инженер</t>
+  </si>
+  <si>
+    <t>Системный администратор</t>
+  </si>
+  <si>
+    <t>Бухгалтер</t>
+  </si>
+  <si>
+    <t>Паркхмахер</t>
+  </si>
+  <si>
+    <t>Диспетчер</t>
+  </si>
+  <si>
+    <t>Оленевод</t>
+  </si>
+  <si>
+    <t>Охраник</t>
+  </si>
+  <si>
+    <t>Директор</t>
+  </si>
+  <si>
+    <t>фамилия</t>
+  </si>
+  <si>
+    <t>отчество</t>
+  </si>
+  <si>
+    <t>возраст</t>
+  </si>
+  <si>
+    <t>телефон</t>
+  </si>
+  <si>
+    <t>улица</t>
+  </si>
+  <si>
+    <t>почта</t>
+  </si>
+  <si>
+    <t>пол</t>
+  </si>
+  <si>
+    <t>паспорт</t>
+  </si>
+  <si>
+    <t>должность</t>
+  </si>
+  <si>
+    <t>имя</t>
   </si>
 </sst>
 </file>
@@ -489,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,56 +530,59 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -558,27 +591,30 @@
         <v>89128976541</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="J2">
         <v>169300</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="M2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -587,27 +623,30 @@
         <v>89047517896</v>
       </c>
       <c r="I3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="J3">
         <v>189500</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>31</v>
@@ -616,24 +655,27 @@
         <v>89121228995</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="J4">
         <v>260800</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>19</v>
@@ -642,24 +684,27 @@
         <v>89123769128</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="J5">
         <v>150970</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>44</v>
@@ -668,21 +713,24 @@
         <v>89046579023</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="M6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
       </c>
       <c r="E7">
         <v>22</v>
@@ -691,21 +739,24 @@
         <v>89128995379</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E8">
         <v>61</v>
@@ -714,21 +765,24 @@
         <v>89123899213</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="M8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <v>15</v>
@@ -737,21 +791,24 @@
         <v>89128234319</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
       </c>
       <c r="E10">
         <v>33</v>
@@ -760,7 +817,10 @@
         <v>89128975273</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>37</v>
+      </c>
+      <c r="M10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed name of EntityOf. Collect all entities to complex map and fill it by excel data.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/data.xlsx
+++ b/src/main/resources/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ДИПЛОМ\SpringDiploma\ustu\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8DFA3D-5A8B-4694-8A64-14A3012B766D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929953D8-A5DF-44BE-A6C9-74C763E2AEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3072" yWindow="1572" windowWidth="17280" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>имя</t>
+  </si>
+  <si>
+    <t>корпорация</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Tesla</t>
+  </si>
+  <si>
+    <t>SpaceX</t>
   </si>
 </sst>
 </file>
@@ -519,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +542,7 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,8 +582,11 @@
       <c r="M1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -602,8 +617,11 @@
       <c r="M2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -634,8 +652,11 @@
       <c r="M3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -663,8 +684,11 @@
       <c r="M4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -693,7 +717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -719,7 +743,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -745,7 +769,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -771,7 +795,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -797,7 +821,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>

</xml_diff>